<commit_message>
added DU to bha for yetweyntwe
</commit_message>
<xml_diff>
--- a/data/rules.xlsx
+++ b/data/rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergeimalyshev/Desktop/Tocharian/Tocharian A/My grammar/Candrakanta/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E5886E-4F08-0F42-87FC-D84B3707B463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1571D4CD-8A42-7B42-BDA0-1D7BDDADCB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="580" windowWidth="29920" windowHeight="14180" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
+    <workbookView xWindow="0" yWindow="580" windowWidth="29920" windowHeight="14180" xr2:uid="{DFFD3512-190B-6C44-A03E-FE8C03207A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="3" r:id="rId1"/>
@@ -10391,10 +10391,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF76C2B-797E-2544-85E2-CF60CE11F59B}">
   <dimension ref="A1:XFA772"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" zoomScale="177" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A666" zoomScale="177" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A651" sqref="A651"/>
-      <selection pane="topRight" activeCell="C674" sqref="C674"/>
+      <selection pane="topRight" activeCell="F677" sqref="F677"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>